<commit_message>
Add : Created All Model's Traits and Attributes Maker. Todo : Set Name -> npc, pet, item , equipment, achievement
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Effects/Resources/Documents/Ability/StatusesInfo.xlsx
+++ b/Assets/Scripts/1.Abilities/Effects/Resources/Documents/Ability/StatusesInfo.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Effects\Resources\Documents\Ability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BackUp 2023-0324\Unity Portfolios\BoilerPlate\BP\Assets\Scripts\1.Abilities\Effects\Resources\Documents\Ability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF68ABBF-0EF4-44B5-8597-026291A8A0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B53CB-BF05-4536-95B7-2F18158592DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32745" yWindow="3435" windowWidth="28785" windowHeight="15345" activeTab="1" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
+    <workbookView xWindow="11430" yWindow="7140" windowWidth="24900" windowHeight="11860" activeTab="4" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="8" r:id="rId1"/>
     <sheet name="StatusTypes" sheetId="11" r:id="rId2"/>
     <sheet name="StatusesBase" sheetId="9" r:id="rId3"/>
-    <sheet name="BattleStatuses" sheetId="3" r:id="rId4"/>
-    <sheet name="LifeStatuses" sheetId="10" r:id="rId5"/>
+    <sheet name="NpcStatuses" sheetId="3" r:id="rId4"/>
+    <sheet name="ItemStatuses" sheetId="13" r:id="rId5"/>
+    <sheet name="EquipmentStatuses" sheetId="10" r:id="rId6"/>
+    <sheet name="PetStatuses" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="205">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -848,6 +850,14 @@
   </si>
   <si>
     <t>BattleBehaviour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오크</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1236,9 +1246,9 @@
       <selection activeCell="F1" sqref="F1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1260,84 +1270,84 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="F13:H13"/>
@@ -1366,13 +1376,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0559C2D4-7B33-4877-A3EC-84D656755EE2}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>196</v>
       </c>
@@ -1389,7 +1399,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>188</v>
       </c>
@@ -1406,7 +1416,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -1420,7 +1430,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -1434,7 +1444,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -1442,7 +1452,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>194</v>
       </c>
@@ -1450,7 +1460,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -1458,7 +1468,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>192</v>
       </c>
@@ -1477,9 +1487,9 @@
       <selection activeCell="F63" sqref="F63:H63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1507,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1515,7 +1525,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1543,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1561,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -1569,7 +1579,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>94</v>
       </c>
@@ -1587,7 +1597,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1605,7 +1615,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
@@ -1623,7 +1633,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>95</v>
       </c>
@@ -1641,7 +1651,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1659,7 +1669,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>77</v>
       </c>
@@ -1677,7 +1687,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>96</v>
       </c>
@@ -1695,7 +1705,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1713,7 +1723,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1731,7 +1741,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1749,7 +1759,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1767,7 +1777,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1785,7 +1795,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1803,7 +1813,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -1821,7 +1831,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1839,7 +1849,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1857,7 +1867,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -1875,7 +1885,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
@@ -1893,7 +1903,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1911,7 +1921,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
@@ -1929,7 +1939,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>37</v>
       </c>
@@ -1947,7 +1957,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
@@ -1965,7 +1975,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
@@ -1983,7 +1993,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
@@ -2001,7 +2011,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -2019,7 +2029,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -2037,7 +2047,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
@@ -2055,7 +2065,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>54</v>
       </c>
@@ -2073,7 +2083,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
@@ -2091,7 +2101,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>58</v>
       </c>
@@ -2109,7 +2119,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
@@ -2127,7 +2137,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>62</v>
       </c>
@@ -2145,7 +2155,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -2163,7 +2173,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -2181,7 +2191,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>71</v>
       </c>
@@ -2199,7 +2209,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>72</v>
       </c>
@@ -2217,7 +2227,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>79</v>
       </c>
@@ -2235,7 +2245,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>80</v>
       </c>
@@ -2253,7 +2263,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>84</v>
       </c>
@@ -2271,7 +2281,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>85</v>
       </c>
@@ -2289,7 +2299,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>86</v>
       </c>
@@ -2307,7 +2317,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>100</v>
       </c>
@@ -2325,7 +2335,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>101</v>
       </c>
@@ -2343,7 +2353,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>102</v>
       </c>
@@ -2361,7 +2371,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>103</v>
       </c>
@@ -2379,7 +2389,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>110</v>
       </c>
@@ -2397,7 +2407,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>111</v>
       </c>
@@ -2415,7 +2425,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
@@ -2433,7 +2443,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>113</v>
       </c>
@@ -2451,7 +2461,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>118</v>
       </c>
@@ -2469,7 +2479,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>119</v>
       </c>
@@ -2487,7 +2497,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>122</v>
       </c>
@@ -2505,7 +2515,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>123</v>
       </c>
@@ -2523,7 +2533,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>108</v>
       </c>
@@ -2541,7 +2551,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>126</v>
       </c>
@@ -2559,7 +2569,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>129</v>
       </c>
@@ -2577,7 +2587,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>131</v>
       </c>
@@ -2595,7 +2605,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>109</v>
       </c>
@@ -2613,55 +2623,122 @@
     </row>
   </sheetData>
   <mergeCells count="189">
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>
@@ -2686,122 +2763,55 @@
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2813,12 +2823,12 @@
   <dimension ref="A1:BJ5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3006,7 +3016,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3194,7 +3204,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3258,7 +3268,7 @@
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -3275,58 +3285,12 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
     <mergeCell ref="BI2:BI3"/>
     <mergeCell ref="BH2:BH3"/>
     <mergeCell ref="BJ2:BJ3"/>
@@ -3343,6 +3307,52 @@
     <mergeCell ref="AT2:AT3"/>
     <mergeCell ref="AU2:AU3"/>
     <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3350,13 +3360,1623 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E342C21-B894-4AC4-8AA4-C156F8E0A45D}">
+  <dimension ref="A1:BJ5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="62">
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="BE2:BE3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9F6E95-6F19-40B6-AADC-527FB42B88D1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BJ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="62">
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="BE2:BE3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C15347-A30D-4A4F-B512-2D62829FEA4F}">
+  <dimension ref="A1:BJ5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>118</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="62">
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="BE2:BE3"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Divide Growable, Enhancable, Combinable Add Create Growable, Enhancable, Combinable Todo ::
 1. Clear - Nested Command
 2. Save & Load
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Effects/Resources/Documents/Ability/StatusesInfo.xlsx
+++ b/Assets/Scripts/1.Abilities/Effects/Resources/Documents/Ability/StatusesInfo.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BackUp 2023-0324\Unity Portfolios\BoilerPlate\BP\Assets\Scripts\1.Abilities\Effects\Resources\Documents\Ability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B53CB-BF05-4536-95B7-2F18158592DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9DF965-1F31-41CF-B237-2AC77EA556FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="7140" windowWidth="24900" windowHeight="11860" activeTab="4" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
+    <workbookView xWindow="10930" yWindow="3280" windowWidth="24900" windowHeight="16010" firstSheet="2" activeTab="4" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="8" r:id="rId1"/>
-    <sheet name="StatusTypes" sheetId="11" r:id="rId2"/>
-    <sheet name="StatusesBase" sheetId="9" r:id="rId3"/>
-    <sheet name="NpcStatuses" sheetId="3" r:id="rId4"/>
-    <sheet name="ItemStatuses" sheetId="13" r:id="rId5"/>
-    <sheet name="EquipmentStatuses" sheetId="10" r:id="rId6"/>
-    <sheet name="PetStatuses" sheetId="12" r:id="rId7"/>
+    <sheet name="Enhancable" sheetId="15" r:id="rId2"/>
+    <sheet name="StatusTypes" sheetId="11" r:id="rId3"/>
+    <sheet name="StatusesBase" sheetId="9" r:id="rId4"/>
+    <sheet name="NpcStatuses" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="204">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -853,11 +851,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>단검</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오크</t>
+    <t>Achievement</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1373,16 +1367,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A869D67C-64C1-4B81-9EB0-6052661E6916}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0559C2D4-7B33-4877-A3EC-84D656755EE2}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>196</v>
       </c>
@@ -1398,8 +1405,11 @@
       <c r="E1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>188</v>
       </c>
@@ -1415,8 +1425,11 @@
       <c r="E2" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -1429,8 +1442,11 @@
       <c r="D3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -1443,8 +1459,11 @@
       <c r="D4" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>193</v>
       </c>
@@ -1452,7 +1471,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>194</v>
       </c>
@@ -1460,7 +1479,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>195</v>
       </c>
@@ -1468,7 +1487,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>192</v>
       </c>
@@ -1479,12 +1498,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232347A5-EE01-4595-94B7-E44C62186A2E}">
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F63" sqref="F63:H63"/>
+      <selection activeCell="F14" sqref="F14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2818,12 +2837,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{965D1BFB-24F6-48A0-A008-1A4B0B7A7FCD}">
   <dimension ref="A1:BJ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3327,6 +3346,8 @@
     <mergeCell ref="Y2:Y3"/>
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="AM2:AM3"/>
     <mergeCell ref="AN2:AN3"/>
     <mergeCell ref="AO2:AO3"/>
@@ -3335,8 +3356,6 @@
     <mergeCell ref="AH2:AH3"/>
     <mergeCell ref="AI2:AI3"/>
     <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="L2:L3"/>
@@ -3357,1627 +3376,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E342C21-B894-4AC4-8AA4-C156F8E0A45D}">
-  <dimension ref="A1:BJ5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>129</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="2"/>
-      <c r="BF3" s="2"/>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
-    </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="BE2:BE3"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9F6E95-6F19-40B6-AADC-527FB42B88D1}">
-  <dimension ref="A1:BJ5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>129</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="2"/>
-      <c r="BF3" s="2"/>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
-    </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="BE2:BE3"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C15347-A30D-4A4F-B512-2D62829FEA4F}">
-  <dimension ref="A1:BJ5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" t="s">
-        <v>39</v>
-      </c>
-      <c r="X1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>123</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>126</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>129</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>131</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2"/>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2"/>
-      <c r="AY3" s="2"/>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2"/>
-      <c r="BE3" s="2"/>
-      <c r="BF3" s="2"/>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
-    </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.45">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="BE2:BE3"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>